<commit_message>
List of all the processed movies.
</commit_message>
<xml_diff>
--- a/analysisLog.xlsx
+++ b/analysisLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\utkarsh\Projects\mof-radiation-damage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66B481E-599F-4FA7-B19B-0A0ACF22FA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA2C4DA-3DC8-4FD2-8F86-AFACDDE3FA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProcessedMovies" sheetId="1" r:id="rId1"/>
@@ -1476,7 +1476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add new sheet with cumulative decay dose.
</commit_message>
<xml_diff>
--- a/analysisLog.xlsx
+++ b/analysisLog.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\utkarsh\Projects\mof-radiation-damage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA2C4DA-3DC8-4FD2-8F86-AFACDDE3FA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3339342-CAF5-47B2-8911-2DCFB8F1D675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="0" windowWidth="22540" windowHeight="14440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProcessedMovies" sheetId="1" r:id="rId1"/>
     <sheet name="AllMovies" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="68">
   <si>
     <t>Input directory</t>
   </si>
@@ -221,13 +222,22 @@
   </si>
   <si>
     <t>/scratch/utkur/utkarsh/MOFDecay/298K/SAA1/J_1.00/20210510/002</t>
+  </si>
+  <si>
+    <t>Movie</t>
+  </si>
+  <si>
+    <t>Minimum OP</t>
+  </si>
+  <si>
+    <t>Reject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -243,6 +253,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -252,7 +276,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -260,13 +284,211 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,7 +805,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1476,9 +1700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D67"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2361,4 +2583,1028 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2F8691-40A6-466B-A544-E902567AC361}">
+  <dimension ref="A1:K63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="14"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="11">
+        <v>150</v>
+      </c>
+      <c r="C2" s="11">
+        <v>250</v>
+      </c>
+      <c r="D2" s="11">
+        <v>350</v>
+      </c>
+      <c r="E2" s="11">
+        <v>450</v>
+      </c>
+      <c r="F2" s="11">
+        <v>550</v>
+      </c>
+      <c r="G2" s="11">
+        <v>650</v>
+      </c>
+      <c r="H2" s="11">
+        <v>750</v>
+      </c>
+      <c r="I2" s="11">
+        <v>850</v>
+      </c>
+      <c r="J2" s="11">
+        <v>950</v>
+      </c>
+      <c r="K2" s="12">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9">
+        <v>5644</v>
+      </c>
+      <c r="C3" s="9">
+        <v>4140</v>
+      </c>
+      <c r="D3" s="17">
+        <v>2872</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1794</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>1517</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1134</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2504</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1228</v>
+      </c>
+      <c r="D5" s="2">
+        <v>928</v>
+      </c>
+      <c r="E5" s="2">
+        <v>388</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>291</v>
+      </c>
+      <c r="C7" s="2">
+        <v>107</v>
+      </c>
+      <c r="D7" s="2">
+        <v>73</v>
+      </c>
+      <c r="E7" s="2">
+        <v>47</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="3"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="3"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="3"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>